<commit_message>
chore: update geo-ip data - 20250912_133152
📊 Data sync summary:
- Updated at: 2025-09-12 13:31:54 UTC
- Territories: 250
- IP ranges: 258299
- Data size: 41.20MB

🤖 Auto-generated by GitHub Actions
</commit_message>
<xml_diff>
--- a/data/combined-geo-ip-data.xlsx
+++ b/data/combined-geo-ip-data.xlsx
@@ -22,7 +22,7 @@
     <t>Generated at:</t>
   </si>
   <si>
-    <t>2025-08-12T03:16:22.102Z</t>
+    <t>2025-09-12T13:30:06.263Z</t>
   </si>
   <si>
     <t>Metric</t>
@@ -3172,7 +3172,7 @@
     <t>IP Ranges Data Too Large</t>
   </si>
   <si>
-    <t>Total IP ranges: 256807</t>
+    <t>Total IP ranges: 258299</t>
   </si>
   <si>
     <t>The IP ranges data is too large to include in Excel format.</t>
@@ -3661,7 +3661,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>256807</v>
+        <v>258299</v>
       </c>
     </row>
   </sheetData>
@@ -3743,7 +3743,7 @@
         <v>25</v>
       </c>
       <c r="I2">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -3772,7 +3772,7 @@
         <v>25</v>
       </c>
       <c r="I3">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -3801,7 +3801,7 @@
         <v>25</v>
       </c>
       <c r="I4">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -3859,7 +3859,7 @@
         <v>25</v>
       </c>
       <c r="I6">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -3888,7 +3888,7 @@
         <v>25</v>
       </c>
       <c r="I7">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3946,7 +3946,7 @@
         <v>44</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -3975,7 +3975,7 @@
         <v>25</v>
       </c>
       <c r="I10">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -4004,7 +4004,7 @@
         <v>25</v>
       </c>
       <c r="I11">
-        <v>1859</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -4033,7 +4033,7 @@
         <v>25</v>
       </c>
       <c r="I12">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -4091,7 +4091,7 @@
         <v>25</v>
       </c>
       <c r="I14">
-        <v>7238</v>
+        <v>7251</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -4120,7 +4120,7 @@
         <v>25</v>
       </c>
       <c r="I15">
-        <v>2313</v>
+        <v>2322</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -4149,7 +4149,7 @@
         <v>25</v>
       </c>
       <c r="I16">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -4178,7 +4178,7 @@
         <v>25</v>
       </c>
       <c r="I17">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -4207,7 +4207,7 @@
         <v>25</v>
       </c>
       <c r="I18">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -4236,7 +4236,7 @@
         <v>25</v>
       </c>
       <c r="I19">
-        <v>1973</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -4265,7 +4265,7 @@
         <v>25</v>
       </c>
       <c r="I20">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -4294,7 +4294,7 @@
         <v>25</v>
       </c>
       <c r="I21">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -4323,7 +4323,7 @@
         <v>25</v>
       </c>
       <c r="I22">
-        <v>4930</v>
+        <v>5035</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -4352,7 +4352,7 @@
         <v>25</v>
       </c>
       <c r="I23">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -4410,7 +4410,7 @@
         <v>44</v>
       </c>
       <c r="I25">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -4439,7 +4439,7 @@
         <v>25</v>
       </c>
       <c r="I26">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -4468,7 +4468,7 @@
         <v>25</v>
       </c>
       <c r="I27">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -4497,7 +4497,7 @@
         <v>25</v>
       </c>
       <c r="I28">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -4526,7 +4526,7 @@
         <v>25</v>
       </c>
       <c r="I29">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -4584,7 +4584,7 @@
         <v>25</v>
       </c>
       <c r="I31">
-        <v>4802</v>
+        <v>4790</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -4642,7 +4642,7 @@
         <v>44</v>
       </c>
       <c r="I33">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -4671,7 +4671,7 @@
         <v>25</v>
       </c>
       <c r="I34">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -4729,7 +4729,7 @@
         <v>25</v>
       </c>
       <c r="I36">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -4758,7 +4758,7 @@
         <v>25</v>
       </c>
       <c r="I37">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -4787,7 +4787,7 @@
         <v>25</v>
       </c>
       <c r="I38">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -4845,7 +4845,7 @@
         <v>25</v>
       </c>
       <c r="I40">
-        <v>8788</v>
+        <v>8731</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -4903,7 +4903,7 @@
         <v>44</v>
       </c>
       <c r="I42">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -4932,7 +4932,7 @@
         <v>44</v>
       </c>
       <c r="I43">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -4961,7 +4961,7 @@
         <v>25</v>
       </c>
       <c r="I44">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -5019,7 +5019,7 @@
         <v>25</v>
       </c>
       <c r="I46">
-        <v>1014</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -5048,7 +5048,7 @@
         <v>25</v>
       </c>
       <c r="I47">
-        <v>4422</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -5135,7 +5135,7 @@
         <v>25</v>
       </c>
       <c r="I50">
-        <v>1039</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -5193,7 +5193,7 @@
         <v>25</v>
       </c>
       <c r="I52">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -5222,7 +5222,7 @@
         <v>44</v>
       </c>
       <c r="I53">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -5251,7 +5251,7 @@
         <v>25</v>
       </c>
       <c r="I54">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -5280,7 +5280,7 @@
         <v>25</v>
       </c>
       <c r="I55">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -5338,7 +5338,7 @@
         <v>44</v>
       </c>
       <c r="I57">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -5367,7 +5367,7 @@
         <v>25</v>
       </c>
       <c r="I58">
-        <v>337</v>
+        <v>342</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -5396,7 +5396,7 @@
         <v>25</v>
       </c>
       <c r="I59">
-        <v>1883</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -5425,7 +5425,7 @@
         <v>25</v>
       </c>
       <c r="I60">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -5454,7 +5454,7 @@
         <v>25</v>
       </c>
       <c r="I61">
-        <v>1601</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -5483,7 +5483,7 @@
         <v>25</v>
       </c>
       <c r="I62">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -5512,7 +5512,7 @@
         <v>25</v>
       </c>
       <c r="I63">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -5541,7 +5541,7 @@
         <v>25</v>
       </c>
       <c r="I64">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -5570,7 +5570,7 @@
         <v>25</v>
       </c>
       <c r="I65">
-        <v>465</v>
+        <v>448</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -5599,7 +5599,7 @@
         <v>25</v>
       </c>
       <c r="I66">
-        <v>298</v>
+        <v>310</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -5628,7 +5628,7 @@
         <v>25</v>
       </c>
       <c r="I67">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -5686,7 +5686,7 @@
         <v>25</v>
       </c>
       <c r="I69">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -5715,7 +5715,7 @@
         <v>25</v>
       </c>
       <c r="I70">
-        <v>658</v>
+        <v>676</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -5889,7 +5889,7 @@
         <v>25</v>
       </c>
       <c r="I76">
-        <v>1845</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -5918,7 +5918,7 @@
         <v>25</v>
       </c>
       <c r="I77">
-        <v>8795</v>
+        <v>8769</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -5976,7 +5976,7 @@
         <v>44</v>
       </c>
       <c r="I79">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -6034,7 +6034,7 @@
         <v>25</v>
       </c>
       <c r="I81">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -6092,7 +6092,7 @@
         <v>25</v>
       </c>
       <c r="I83">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -6121,7 +6121,7 @@
         <v>25</v>
       </c>
       <c r="I84">
-        <v>14968</v>
+        <v>15357</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -6150,7 +6150,7 @@
         <v>25</v>
       </c>
       <c r="I85">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -6208,7 +6208,7 @@
         <v>25</v>
       </c>
       <c r="I87">
-        <v>685</v>
+        <v>695</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -6237,7 +6237,7 @@
         <v>44</v>
       </c>
       <c r="I88">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -6266,7 +6266,7 @@
         <v>25</v>
       </c>
       <c r="I89">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -6295,7 +6295,7 @@
         <v>44</v>
       </c>
       <c r="I90">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -6324,7 +6324,7 @@
         <v>44</v>
       </c>
       <c r="I91">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -6353,7 +6353,7 @@
         <v>25</v>
       </c>
       <c r="I92">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -6382,7 +6382,7 @@
         <v>44</v>
       </c>
       <c r="I93">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -6411,7 +6411,7 @@
         <v>25</v>
       </c>
       <c r="I94">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -6440,7 +6440,7 @@
         <v>25</v>
       </c>
       <c r="I95">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -6469,7 +6469,7 @@
         <v>25</v>
       </c>
       <c r="I96">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -6498,7 +6498,7 @@
         <v>25</v>
       </c>
       <c r="I97">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -6556,7 +6556,7 @@
         <v>25</v>
       </c>
       <c r="I99">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -6585,7 +6585,7 @@
         <v>44</v>
       </c>
       <c r="I100">
-        <v>6500</v>
+        <v>6759</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -6614,7 +6614,7 @@
         <v>25</v>
       </c>
       <c r="I101">
-        <v>937</v>
+        <v>922</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -6672,7 +6672,7 @@
         <v>25</v>
       </c>
       <c r="I103">
-        <v>7778</v>
+        <v>7714</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -6701,7 +6701,7 @@
         <v>25</v>
       </c>
       <c r="I104">
-        <v>4407</v>
+        <v>4474</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
@@ -6730,7 +6730,7 @@
         <v>25</v>
       </c>
       <c r="I105">
-        <v>1605</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
@@ -6759,7 +6759,7 @@
         <v>25</v>
       </c>
       <c r="I106">
-        <v>383</v>
+        <v>388</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -6788,7 +6788,7 @@
         <v>25</v>
       </c>
       <c r="I107">
-        <v>2220</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -6817,7 +6817,7 @@
         <v>44</v>
       </c>
       <c r="I108">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
@@ -6846,7 +6846,7 @@
         <v>25</v>
       </c>
       <c r="I109">
-        <v>1178</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -6875,7 +6875,7 @@
         <v>25</v>
       </c>
       <c r="I110">
-        <v>4977</v>
+        <v>5032</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
@@ -6904,7 +6904,7 @@
         <v>25</v>
       </c>
       <c r="I111">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -6933,7 +6933,7 @@
         <v>25</v>
       </c>
       <c r="I112">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
@@ -6962,7 +6962,7 @@
         <v>25</v>
       </c>
       <c r="I113">
-        <v>6570</v>
+        <v>6603</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
@@ -6991,7 +6991,7 @@
         <v>44</v>
       </c>
       <c r="I114">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -7020,7 +7020,7 @@
         <v>25</v>
       </c>
       <c r="I115">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -7049,7 +7049,7 @@
         <v>25</v>
       </c>
       <c r="I116">
-        <v>893</v>
+        <v>907</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -7078,7 +7078,7 @@
         <v>25</v>
       </c>
       <c r="I117">
-        <v>488</v>
+        <v>492</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -7107,7 +7107,7 @@
         <v>25</v>
       </c>
       <c r="I118">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -7165,7 +7165,7 @@
         <v>25</v>
       </c>
       <c r="I120">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -7194,7 +7194,7 @@
         <v>25</v>
       </c>
       <c r="I121">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
@@ -7223,7 +7223,7 @@
         <v>25</v>
       </c>
       <c r="I122">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
@@ -7252,7 +7252,7 @@
         <v>25</v>
       </c>
       <c r="I123">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
@@ -7281,7 +7281,7 @@
         <v>25</v>
       </c>
       <c r="I124">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
@@ -7339,7 +7339,7 @@
         <v>25</v>
       </c>
       <c r="I126">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
@@ -7397,7 +7397,7 @@
         <v>25</v>
       </c>
       <c r="I128">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -7426,7 +7426,7 @@
         <v>25</v>
       </c>
       <c r="I129">
-        <v>894</v>
+        <v>857</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -7455,7 +7455,7 @@
         <v>25</v>
       </c>
       <c r="I130">
-        <v>554</v>
+        <v>545</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
@@ -7513,7 +7513,7 @@
         <v>25</v>
       </c>
       <c r="I132">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
@@ -7542,7 +7542,7 @@
         <v>25</v>
       </c>
       <c r="I133">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
@@ -7571,7 +7571,7 @@
         <v>25</v>
       </c>
       <c r="I134">
-        <v>1433</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
@@ -7600,7 +7600,7 @@
         <v>25</v>
       </c>
       <c r="I135">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
@@ -7629,7 +7629,7 @@
         <v>25</v>
       </c>
       <c r="I136">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
@@ -7658,7 +7658,7 @@
         <v>25</v>
       </c>
       <c r="I137">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
@@ -7687,7 +7687,7 @@
         <v>25</v>
       </c>
       <c r="I138">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
@@ -7832,7 +7832,7 @@
         <v>25</v>
       </c>
       <c r="I143">
-        <v>1611</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
@@ -7861,7 +7861,7 @@
         <v>25</v>
       </c>
       <c r="I144">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
@@ -7890,7 +7890,7 @@
         <v>25</v>
       </c>
       <c r="I145">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
@@ -7919,7 +7919,7 @@
         <v>25</v>
       </c>
       <c r="I146">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
@@ -7977,7 +7977,7 @@
         <v>25</v>
       </c>
       <c r="I148">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
@@ -8006,7 +8006,7 @@
         <v>44</v>
       </c>
       <c r="I149">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
@@ -8035,7 +8035,7 @@
         <v>25</v>
       </c>
       <c r="I150">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
@@ -8064,7 +8064,7 @@
         <v>25</v>
       </c>
       <c r="I151">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
@@ -8093,7 +8093,7 @@
         <v>25</v>
       </c>
       <c r="I152">
-        <v>287</v>
+        <v>294</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
@@ -8122,7 +8122,7 @@
         <v>25</v>
       </c>
       <c r="I153">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
@@ -8180,7 +8180,7 @@
         <v>25</v>
       </c>
       <c r="I155">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
@@ -8209,7 +8209,7 @@
         <v>25</v>
       </c>
       <c r="I156">
-        <v>10776</v>
+        <v>10629</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
@@ -8238,7 +8238,7 @@
         <v>44</v>
       </c>
       <c r="I157">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
@@ -8267,7 +8267,7 @@
         <v>25</v>
       </c>
       <c r="I158">
-        <v>1504</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
@@ -8296,7 +8296,7 @@
         <v>25</v>
       </c>
       <c r="I159">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
@@ -8354,7 +8354,7 @@
         <v>25</v>
       </c>
       <c r="I161">
-        <v>507</v>
+        <v>522</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
@@ -8470,7 +8470,7 @@
         <v>25</v>
       </c>
       <c r="I165">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
@@ -8499,7 +8499,7 @@
         <v>44</v>
       </c>
       <c r="I166">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
@@ -8528,7 +8528,7 @@
         <v>25</v>
       </c>
       <c r="I167">
-        <v>1657</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
@@ -8557,7 +8557,7 @@
         <v>25</v>
       </c>
       <c r="I168">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
@@ -8586,7 +8586,7 @@
         <v>25</v>
       </c>
       <c r="I169">
-        <v>841</v>
+        <v>847</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
@@ -8615,7 +8615,7 @@
         <v>25</v>
       </c>
       <c r="I170">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
@@ -8644,7 +8644,7 @@
         <v>44</v>
       </c>
       <c r="I171">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
@@ -8673,7 +8673,7 @@
         <v>25</v>
       </c>
       <c r="I172">
-        <v>325</v>
+        <v>316</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
@@ -8702,7 +8702,7 @@
         <v>25</v>
       </c>
       <c r="I173">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
@@ -8731,7 +8731,7 @@
         <v>25</v>
       </c>
       <c r="I174">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
@@ -8760,7 +8760,7 @@
         <v>25</v>
       </c>
       <c r="I175">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
@@ -8789,7 +8789,7 @@
         <v>25</v>
       </c>
       <c r="I176">
-        <v>1451</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
@@ -8847,7 +8847,7 @@
         <v>25</v>
       </c>
       <c r="I178">
-        <v>4916</v>
+        <v>4923</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
@@ -8876,7 +8876,7 @@
         <v>25</v>
       </c>
       <c r="I179">
-        <v>649</v>
+        <v>661</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
@@ -8905,7 +8905,7 @@
         <v>44</v>
       </c>
       <c r="I180">
-        <v>374</v>
+        <v>357</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
@@ -8934,7 +8934,7 @@
         <v>25</v>
       </c>
       <c r="I181">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
@@ -8963,7 +8963,7 @@
         <v>25</v>
       </c>
       <c r="I182">
-        <v>2469</v>
+        <v>2426</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
@@ -8992,7 +8992,7 @@
         <v>25</v>
       </c>
       <c r="I183">
-        <v>8996</v>
+        <v>9089</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
@@ -9021,7 +9021,7 @@
         <v>25</v>
       </c>
       <c r="I184">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
@@ -9050,7 +9050,7 @@
         <v>44</v>
       </c>
       <c r="I185">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
@@ -9079,7 +9079,7 @@
         <v>44</v>
       </c>
       <c r="I186">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
@@ -9137,7 +9137,7 @@
         <v>25</v>
       </c>
       <c r="I188">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
@@ -9195,7 +9195,7 @@
         <v>44</v>
       </c>
       <c r="I190">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.25">
@@ -9253,7 +9253,7 @@
         <v>25</v>
       </c>
       <c r="I192">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
@@ -9282,7 +9282,7 @@
         <v>25</v>
       </c>
       <c r="I193">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
@@ -9340,7 +9340,7 @@
         <v>25</v>
       </c>
       <c r="I195">
-        <v>885</v>
+        <v>920</v>
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.25">
@@ -9369,7 +9369,7 @@
         <v>25</v>
       </c>
       <c r="I196">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.25">
@@ -9398,7 +9398,7 @@
         <v>25</v>
       </c>
       <c r="I197">
-        <v>574</v>
+        <v>578</v>
       </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.25">
@@ -9427,7 +9427,7 @@
         <v>25</v>
       </c>
       <c r="I198">
-        <v>336</v>
+        <v>296</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.25">
@@ -9456,7 +9456,7 @@
         <v>25</v>
       </c>
       <c r="I199">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.25">
@@ -9485,7 +9485,7 @@
         <v>25</v>
       </c>
       <c r="I200">
-        <v>4872</v>
+        <v>4906</v>
       </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">
@@ -9543,7 +9543,7 @@
         <v>25</v>
       </c>
       <c r="I202">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.25">
@@ -9572,7 +9572,7 @@
         <v>25</v>
       </c>
       <c r="I203">
-        <v>574</v>
+        <v>603</v>
       </c>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
@@ -9601,7 +9601,7 @@
         <v>25</v>
       </c>
       <c r="I204">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.25">
@@ -9630,7 +9630,7 @@
         <v>25</v>
       </c>
       <c r="I205">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.25">
@@ -9659,7 +9659,7 @@
         <v>25</v>
       </c>
       <c r="I206">
-        <v>2316</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.25">
@@ -9717,7 +9717,7 @@
         <v>25</v>
       </c>
       <c r="I208">
-        <v>2275</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.25">
@@ -9746,7 +9746,7 @@
         <v>25</v>
       </c>
       <c r="I209">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.25">
@@ -9775,7 +9775,7 @@
         <v>25</v>
       </c>
       <c r="I210">
-        <v>5118</v>
+        <v>5255</v>
       </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.25">
@@ -9804,7 +9804,7 @@
         <v>25</v>
       </c>
       <c r="I211">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
@@ -9833,7 +9833,7 @@
         <v>25</v>
       </c>
       <c r="I212">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.25">
@@ -9862,7 +9862,7 @@
         <v>25</v>
       </c>
       <c r="I213">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
@@ -9920,7 +9920,7 @@
         <v>25</v>
       </c>
       <c r="I215">
-        <v>3697</v>
+        <v>3645</v>
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.25">
@@ -9949,7 +9949,7 @@
         <v>25</v>
       </c>
       <c r="I216">
-        <v>3398</v>
+        <v>3444</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.25">
@@ -9978,7 +9978,7 @@
         <v>25</v>
       </c>
       <c r="I217">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.25">
@@ -10036,7 +10036,7 @@
         <v>44</v>
       </c>
       <c r="I219">
-        <v>1400</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.25">
@@ -10065,7 +10065,7 @@
         <v>25</v>
       </c>
       <c r="I220">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.25">
@@ -10094,7 +10094,7 @@
         <v>25</v>
       </c>
       <c r="I221">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.25">
@@ -10123,7 +10123,7 @@
         <v>25</v>
       </c>
       <c r="I222">
-        <v>1249</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.25">
@@ -10152,7 +10152,7 @@
         <v>25</v>
       </c>
       <c r="I223">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.25">
@@ -10239,7 +10239,7 @@
         <v>25</v>
       </c>
       <c r="I226">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.25">
@@ -10268,7 +10268,7 @@
         <v>25</v>
       </c>
       <c r="I227">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.25">
@@ -10384,7 +10384,7 @@
         <v>25</v>
       </c>
       <c r="I231">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.25">
@@ -10413,7 +10413,7 @@
         <v>25</v>
       </c>
       <c r="I232">
-        <v>2380</v>
+        <v>2418</v>
       </c>
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.25">
@@ -10471,7 +10471,7 @@
         <v>25</v>
       </c>
       <c r="I234">
-        <v>3578</v>
+        <v>3571</v>
       </c>
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.25">
@@ -10500,7 +10500,7 @@
         <v>25</v>
       </c>
       <c r="I235">
-        <v>989</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.25">
@@ -10529,7 +10529,7 @@
         <v>25</v>
       </c>
       <c r="I236">
-        <v>15847</v>
+        <v>15894</v>
       </c>
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.25">
@@ -10558,7 +10558,7 @@
         <v>25</v>
       </c>
       <c r="I237">
-        <v>41313</v>
+        <v>41554</v>
       </c>
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.25">
@@ -10587,7 +10587,7 @@
         <v>44</v>
       </c>
       <c r="I238">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.25">
@@ -10616,7 +10616,7 @@
         <v>44</v>
       </c>
       <c r="I239">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.25">
@@ -10645,7 +10645,7 @@
         <v>25</v>
       </c>
       <c r="I240">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.25">
@@ -10674,7 +10674,7 @@
         <v>25</v>
       </c>
       <c r="I241">
-        <v>277</v>
+        <v>288</v>
       </c>
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.25">
@@ -10732,7 +10732,7 @@
         <v>25</v>
       </c>
       <c r="I243">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.25">
@@ -10761,7 +10761,7 @@
         <v>25</v>
       </c>
       <c r="I244">
-        <v>475</v>
+        <v>489</v>
       </c>
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.25">
@@ -10790,7 +10790,7 @@
         <v>25</v>
       </c>
       <c r="I245">
-        <v>1340</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.25">
@@ -10877,7 +10877,7 @@
         <v>25</v>
       </c>
       <c r="I248">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.25">
@@ -11111,7 +11111,7 @@
         <v>993</v>
       </c>
       <c r="B13">
-        <v>41313</v>
+        <v>41554</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -11119,7 +11119,7 @@
         <v>989</v>
       </c>
       <c r="B14">
-        <v>15847</v>
+        <v>15894</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -11127,7 +11127,7 @@
         <v>380</v>
       </c>
       <c r="B15">
-        <v>14968</v>
+        <v>15357</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -11135,7 +11135,7 @@
         <v>669</v>
       </c>
       <c r="B16">
-        <v>10776</v>
+        <v>10629</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -11143,7 +11143,7 @@
         <v>777</v>
       </c>
       <c r="B17">
-        <v>8996</v>
+        <v>9089</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -11151,7 +11151,7 @@
         <v>352</v>
       </c>
       <c r="B18">
-        <v>8795</v>
+        <v>8769</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -11159,7 +11159,7 @@
         <v>201</v>
       </c>
       <c r="B19">
-        <v>8788</v>
+        <v>8731</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -11167,7 +11167,7 @@
         <v>457</v>
       </c>
       <c r="B20">
-        <v>7778</v>
+        <v>7714</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -11175,15 +11175,15 @@
         <v>87</v>
       </c>
       <c r="B21">
-        <v>7238</v>
+        <v>7251</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>497</v>
+        <v>445</v>
       </c>
       <c r="B22">
-        <v>6570</v>
+        <v>6759</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: update geo-ip data - 20250912_144025
📊 Data sync summary:
- Updated at: 2025-09-12 14:40:28 UTC
- Territories: 250
- IP ranges: 258299
- Data size: 41.20MB

🤖 Auto-generated by GitHub Actions
</commit_message>
<xml_diff>
--- a/data/combined-geo-ip-data.xlsx
+++ b/data/combined-geo-ip-data.xlsx
@@ -22,7 +22,7 @@
     <t>Generated at:</t>
   </si>
   <si>
-    <t>2025-08-12T03:16:22.102Z</t>
+    <t>2025-09-12T14:38:36.962Z</t>
   </si>
   <si>
     <t>Metric</t>
@@ -3172,7 +3172,7 @@
     <t>IP Ranges Data Too Large</t>
   </si>
   <si>
-    <t>Total IP ranges: 256807</t>
+    <t>Total IP ranges: 258299</t>
   </si>
   <si>
     <t>The IP ranges data is too large to include in Excel format.</t>
@@ -3661,7 +3661,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>256807</v>
+        <v>258299</v>
       </c>
     </row>
   </sheetData>
@@ -3743,7 +3743,7 @@
         <v>25</v>
       </c>
       <c r="I2">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -3772,7 +3772,7 @@
         <v>25</v>
       </c>
       <c r="I3">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -3801,7 +3801,7 @@
         <v>25</v>
       </c>
       <c r="I4">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -3859,7 +3859,7 @@
         <v>25</v>
       </c>
       <c r="I6">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -3888,7 +3888,7 @@
         <v>25</v>
       </c>
       <c r="I7">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3946,7 +3946,7 @@
         <v>44</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -3975,7 +3975,7 @@
         <v>25</v>
       </c>
       <c r="I10">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -4004,7 +4004,7 @@
         <v>25</v>
       </c>
       <c r="I11">
-        <v>1859</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -4033,7 +4033,7 @@
         <v>25</v>
       </c>
       <c r="I12">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -4091,7 +4091,7 @@
         <v>25</v>
       </c>
       <c r="I14">
-        <v>7238</v>
+        <v>7251</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -4120,7 +4120,7 @@
         <v>25</v>
       </c>
       <c r="I15">
-        <v>2313</v>
+        <v>2322</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -4149,7 +4149,7 @@
         <v>25</v>
       </c>
       <c r="I16">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -4178,7 +4178,7 @@
         <v>25</v>
       </c>
       <c r="I17">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -4207,7 +4207,7 @@
         <v>25</v>
       </c>
       <c r="I18">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -4236,7 +4236,7 @@
         <v>25</v>
       </c>
       <c r="I19">
-        <v>1973</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -4265,7 +4265,7 @@
         <v>25</v>
       </c>
       <c r="I20">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -4294,7 +4294,7 @@
         <v>25</v>
       </c>
       <c r="I21">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -4323,7 +4323,7 @@
         <v>25</v>
       </c>
       <c r="I22">
-        <v>4930</v>
+        <v>5035</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -4352,7 +4352,7 @@
         <v>25</v>
       </c>
       <c r="I23">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -4410,7 +4410,7 @@
         <v>44</v>
       </c>
       <c r="I25">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -4439,7 +4439,7 @@
         <v>25</v>
       </c>
       <c r="I26">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -4468,7 +4468,7 @@
         <v>25</v>
       </c>
       <c r="I27">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -4497,7 +4497,7 @@
         <v>25</v>
       </c>
       <c r="I28">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -4526,7 +4526,7 @@
         <v>25</v>
       </c>
       <c r="I29">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -4584,7 +4584,7 @@
         <v>25</v>
       </c>
       <c r="I31">
-        <v>4802</v>
+        <v>4790</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -4642,7 +4642,7 @@
         <v>44</v>
       </c>
       <c r="I33">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -4671,7 +4671,7 @@
         <v>25</v>
       </c>
       <c r="I34">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -4729,7 +4729,7 @@
         <v>25</v>
       </c>
       <c r="I36">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -4758,7 +4758,7 @@
         <v>25</v>
       </c>
       <c r="I37">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -4787,7 +4787,7 @@
         <v>25</v>
       </c>
       <c r="I38">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -4845,7 +4845,7 @@
         <v>25</v>
       </c>
       <c r="I40">
-        <v>8788</v>
+        <v>8731</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -4903,7 +4903,7 @@
         <v>44</v>
       </c>
       <c r="I42">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -4932,7 +4932,7 @@
         <v>44</v>
       </c>
       <c r="I43">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -4961,7 +4961,7 @@
         <v>25</v>
       </c>
       <c r="I44">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -5019,7 +5019,7 @@
         <v>25</v>
       </c>
       <c r="I46">
-        <v>1014</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -5048,7 +5048,7 @@
         <v>25</v>
       </c>
       <c r="I47">
-        <v>4422</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -5135,7 +5135,7 @@
         <v>25</v>
       </c>
       <c r="I50">
-        <v>1039</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -5193,7 +5193,7 @@
         <v>25</v>
       </c>
       <c r="I52">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -5222,7 +5222,7 @@
         <v>44</v>
       </c>
       <c r="I53">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -5251,7 +5251,7 @@
         <v>25</v>
       </c>
       <c r="I54">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -5280,7 +5280,7 @@
         <v>25</v>
       </c>
       <c r="I55">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -5338,7 +5338,7 @@
         <v>44</v>
       </c>
       <c r="I57">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -5367,7 +5367,7 @@
         <v>25</v>
       </c>
       <c r="I58">
-        <v>337</v>
+        <v>342</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -5396,7 +5396,7 @@
         <v>25</v>
       </c>
       <c r="I59">
-        <v>1883</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -5425,7 +5425,7 @@
         <v>25</v>
       </c>
       <c r="I60">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -5454,7 +5454,7 @@
         <v>25</v>
       </c>
       <c r="I61">
-        <v>1601</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -5483,7 +5483,7 @@
         <v>25</v>
       </c>
       <c r="I62">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -5512,7 +5512,7 @@
         <v>25</v>
       </c>
       <c r="I63">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -5541,7 +5541,7 @@
         <v>25</v>
       </c>
       <c r="I64">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -5570,7 +5570,7 @@
         <v>25</v>
       </c>
       <c r="I65">
-        <v>465</v>
+        <v>448</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -5599,7 +5599,7 @@
         <v>25</v>
       </c>
       <c r="I66">
-        <v>298</v>
+        <v>310</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -5628,7 +5628,7 @@
         <v>25</v>
       </c>
       <c r="I67">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -5686,7 +5686,7 @@
         <v>25</v>
       </c>
       <c r="I69">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -5715,7 +5715,7 @@
         <v>25</v>
       </c>
       <c r="I70">
-        <v>658</v>
+        <v>676</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -5889,7 +5889,7 @@
         <v>25</v>
       </c>
       <c r="I76">
-        <v>1845</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -5918,7 +5918,7 @@
         <v>25</v>
       </c>
       <c r="I77">
-        <v>8795</v>
+        <v>8769</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -5976,7 +5976,7 @@
         <v>44</v>
       </c>
       <c r="I79">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -6034,7 +6034,7 @@
         <v>25</v>
       </c>
       <c r="I81">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -6092,7 +6092,7 @@
         <v>25</v>
       </c>
       <c r="I83">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -6121,7 +6121,7 @@
         <v>25</v>
       </c>
       <c r="I84">
-        <v>14968</v>
+        <v>15357</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -6150,7 +6150,7 @@
         <v>25</v>
       </c>
       <c r="I85">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -6208,7 +6208,7 @@
         <v>25</v>
       </c>
       <c r="I87">
-        <v>685</v>
+        <v>695</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -6237,7 +6237,7 @@
         <v>44</v>
       </c>
       <c r="I88">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -6266,7 +6266,7 @@
         <v>25</v>
       </c>
       <c r="I89">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -6295,7 +6295,7 @@
         <v>44</v>
       </c>
       <c r="I90">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -6324,7 +6324,7 @@
         <v>44</v>
       </c>
       <c r="I91">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -6353,7 +6353,7 @@
         <v>25</v>
       </c>
       <c r="I92">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -6382,7 +6382,7 @@
         <v>44</v>
       </c>
       <c r="I93">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -6411,7 +6411,7 @@
         <v>25</v>
       </c>
       <c r="I94">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -6440,7 +6440,7 @@
         <v>25</v>
       </c>
       <c r="I95">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -6469,7 +6469,7 @@
         <v>25</v>
       </c>
       <c r="I96">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -6498,7 +6498,7 @@
         <v>25</v>
       </c>
       <c r="I97">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -6556,7 +6556,7 @@
         <v>25</v>
       </c>
       <c r="I99">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -6585,7 +6585,7 @@
         <v>44</v>
       </c>
       <c r="I100">
-        <v>6500</v>
+        <v>6759</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -6614,7 +6614,7 @@
         <v>25</v>
       </c>
       <c r="I101">
-        <v>937</v>
+        <v>922</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -6672,7 +6672,7 @@
         <v>25</v>
       </c>
       <c r="I103">
-        <v>7778</v>
+        <v>7714</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -6701,7 +6701,7 @@
         <v>25</v>
       </c>
       <c r="I104">
-        <v>4407</v>
+        <v>4474</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
@@ -6730,7 +6730,7 @@
         <v>25</v>
       </c>
       <c r="I105">
-        <v>1605</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
@@ -6759,7 +6759,7 @@
         <v>25</v>
       </c>
       <c r="I106">
-        <v>383</v>
+        <v>388</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -6788,7 +6788,7 @@
         <v>25</v>
       </c>
       <c r="I107">
-        <v>2220</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -6817,7 +6817,7 @@
         <v>44</v>
       </c>
       <c r="I108">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
@@ -6846,7 +6846,7 @@
         <v>25</v>
       </c>
       <c r="I109">
-        <v>1178</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -6875,7 +6875,7 @@
         <v>25</v>
       </c>
       <c r="I110">
-        <v>4977</v>
+        <v>5032</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
@@ -6904,7 +6904,7 @@
         <v>25</v>
       </c>
       <c r="I111">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -6933,7 +6933,7 @@
         <v>25</v>
       </c>
       <c r="I112">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
@@ -6962,7 +6962,7 @@
         <v>25</v>
       </c>
       <c r="I113">
-        <v>6570</v>
+        <v>6603</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
@@ -6991,7 +6991,7 @@
         <v>44</v>
       </c>
       <c r="I114">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -7020,7 +7020,7 @@
         <v>25</v>
       </c>
       <c r="I115">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -7049,7 +7049,7 @@
         <v>25</v>
       </c>
       <c r="I116">
-        <v>893</v>
+        <v>907</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -7078,7 +7078,7 @@
         <v>25</v>
       </c>
       <c r="I117">
-        <v>488</v>
+        <v>492</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -7107,7 +7107,7 @@
         <v>25</v>
       </c>
       <c r="I118">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -7165,7 +7165,7 @@
         <v>25</v>
       </c>
       <c r="I120">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -7194,7 +7194,7 @@
         <v>25</v>
       </c>
       <c r="I121">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
@@ -7223,7 +7223,7 @@
         <v>25</v>
       </c>
       <c r="I122">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
@@ -7252,7 +7252,7 @@
         <v>25</v>
       </c>
       <c r="I123">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
@@ -7281,7 +7281,7 @@
         <v>25</v>
       </c>
       <c r="I124">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
@@ -7339,7 +7339,7 @@
         <v>25</v>
       </c>
       <c r="I126">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
@@ -7397,7 +7397,7 @@
         <v>25</v>
       </c>
       <c r="I128">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -7426,7 +7426,7 @@
         <v>25</v>
       </c>
       <c r="I129">
-        <v>894</v>
+        <v>857</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -7455,7 +7455,7 @@
         <v>25</v>
       </c>
       <c r="I130">
-        <v>554</v>
+        <v>545</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
@@ -7513,7 +7513,7 @@
         <v>25</v>
       </c>
       <c r="I132">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
@@ -7542,7 +7542,7 @@
         <v>25</v>
       </c>
       <c r="I133">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
@@ -7571,7 +7571,7 @@
         <v>25</v>
       </c>
       <c r="I134">
-        <v>1433</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
@@ -7600,7 +7600,7 @@
         <v>25</v>
       </c>
       <c r="I135">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
@@ -7629,7 +7629,7 @@
         <v>25</v>
       </c>
       <c r="I136">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
@@ -7658,7 +7658,7 @@
         <v>25</v>
       </c>
       <c r="I137">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
@@ -7687,7 +7687,7 @@
         <v>25</v>
       </c>
       <c r="I138">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
@@ -7832,7 +7832,7 @@
         <v>25</v>
       </c>
       <c r="I143">
-        <v>1611</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
@@ -7861,7 +7861,7 @@
         <v>25</v>
       </c>
       <c r="I144">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
@@ -7890,7 +7890,7 @@
         <v>25</v>
       </c>
       <c r="I145">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
@@ -7919,7 +7919,7 @@
         <v>25</v>
       </c>
       <c r="I146">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
@@ -7977,7 +7977,7 @@
         <v>25</v>
       </c>
       <c r="I148">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
@@ -8006,7 +8006,7 @@
         <v>44</v>
       </c>
       <c r="I149">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
@@ -8035,7 +8035,7 @@
         <v>25</v>
       </c>
       <c r="I150">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
@@ -8064,7 +8064,7 @@
         <v>25</v>
       </c>
       <c r="I151">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
@@ -8093,7 +8093,7 @@
         <v>25</v>
       </c>
       <c r="I152">
-        <v>287</v>
+        <v>294</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
@@ -8122,7 +8122,7 @@
         <v>25</v>
       </c>
       <c r="I153">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
@@ -8180,7 +8180,7 @@
         <v>25</v>
       </c>
       <c r="I155">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
@@ -8209,7 +8209,7 @@
         <v>25</v>
       </c>
       <c r="I156">
-        <v>10776</v>
+        <v>10629</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
@@ -8238,7 +8238,7 @@
         <v>44</v>
       </c>
       <c r="I157">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
@@ -8267,7 +8267,7 @@
         <v>25</v>
       </c>
       <c r="I158">
-        <v>1504</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
@@ -8296,7 +8296,7 @@
         <v>25</v>
       </c>
       <c r="I159">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
@@ -8354,7 +8354,7 @@
         <v>25</v>
       </c>
       <c r="I161">
-        <v>507</v>
+        <v>522</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
@@ -8470,7 +8470,7 @@
         <v>25</v>
       </c>
       <c r="I165">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
@@ -8499,7 +8499,7 @@
         <v>44</v>
       </c>
       <c r="I166">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
@@ -8528,7 +8528,7 @@
         <v>25</v>
       </c>
       <c r="I167">
-        <v>1657</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
@@ -8557,7 +8557,7 @@
         <v>25</v>
       </c>
       <c r="I168">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
@@ -8586,7 +8586,7 @@
         <v>25</v>
       </c>
       <c r="I169">
-        <v>841</v>
+        <v>847</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
@@ -8615,7 +8615,7 @@
         <v>25</v>
       </c>
       <c r="I170">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
@@ -8644,7 +8644,7 @@
         <v>44</v>
       </c>
       <c r="I171">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
@@ -8673,7 +8673,7 @@
         <v>25</v>
       </c>
       <c r="I172">
-        <v>325</v>
+        <v>316</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
@@ -8702,7 +8702,7 @@
         <v>25</v>
       </c>
       <c r="I173">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
@@ -8731,7 +8731,7 @@
         <v>25</v>
       </c>
       <c r="I174">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
@@ -8760,7 +8760,7 @@
         <v>25</v>
       </c>
       <c r="I175">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
@@ -8789,7 +8789,7 @@
         <v>25</v>
       </c>
       <c r="I176">
-        <v>1451</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
@@ -8847,7 +8847,7 @@
         <v>25</v>
       </c>
       <c r="I178">
-        <v>4916</v>
+        <v>4923</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
@@ -8876,7 +8876,7 @@
         <v>25</v>
       </c>
       <c r="I179">
-        <v>649</v>
+        <v>661</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
@@ -8905,7 +8905,7 @@
         <v>44</v>
       </c>
       <c r="I180">
-        <v>374</v>
+        <v>357</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
@@ -8934,7 +8934,7 @@
         <v>25</v>
       </c>
       <c r="I181">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
@@ -8963,7 +8963,7 @@
         <v>25</v>
       </c>
       <c r="I182">
-        <v>2469</v>
+        <v>2426</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
@@ -8992,7 +8992,7 @@
         <v>25</v>
       </c>
       <c r="I183">
-        <v>8996</v>
+        <v>9089</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
@@ -9021,7 +9021,7 @@
         <v>25</v>
       </c>
       <c r="I184">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
@@ -9050,7 +9050,7 @@
         <v>44</v>
       </c>
       <c r="I185">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
@@ -9079,7 +9079,7 @@
         <v>44</v>
       </c>
       <c r="I186">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
@@ -9137,7 +9137,7 @@
         <v>25</v>
       </c>
       <c r="I188">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
@@ -9195,7 +9195,7 @@
         <v>44</v>
       </c>
       <c r="I190">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.25">
@@ -9253,7 +9253,7 @@
         <v>25</v>
       </c>
       <c r="I192">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
@@ -9282,7 +9282,7 @@
         <v>25</v>
       </c>
       <c r="I193">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
@@ -9340,7 +9340,7 @@
         <v>25</v>
       </c>
       <c r="I195">
-        <v>885</v>
+        <v>920</v>
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.25">
@@ -9369,7 +9369,7 @@
         <v>25</v>
       </c>
       <c r="I196">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.25">
@@ -9398,7 +9398,7 @@
         <v>25</v>
       </c>
       <c r="I197">
-        <v>574</v>
+        <v>578</v>
       </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.25">
@@ -9427,7 +9427,7 @@
         <v>25</v>
       </c>
       <c r="I198">
-        <v>336</v>
+        <v>296</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.25">
@@ -9456,7 +9456,7 @@
         <v>25</v>
       </c>
       <c r="I199">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.25">
@@ -9485,7 +9485,7 @@
         <v>25</v>
       </c>
       <c r="I200">
-        <v>4872</v>
+        <v>4906</v>
       </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">
@@ -9543,7 +9543,7 @@
         <v>25</v>
       </c>
       <c r="I202">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.25">
@@ -9572,7 +9572,7 @@
         <v>25</v>
       </c>
       <c r="I203">
-        <v>574</v>
+        <v>603</v>
       </c>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
@@ -9601,7 +9601,7 @@
         <v>25</v>
       </c>
       <c r="I204">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.25">
@@ -9630,7 +9630,7 @@
         <v>25</v>
       </c>
       <c r="I205">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.25">
@@ -9659,7 +9659,7 @@
         <v>25</v>
       </c>
       <c r="I206">
-        <v>2316</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.25">
@@ -9717,7 +9717,7 @@
         <v>25</v>
       </c>
       <c r="I208">
-        <v>2275</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.25">
@@ -9746,7 +9746,7 @@
         <v>25</v>
       </c>
       <c r="I209">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.25">
@@ -9775,7 +9775,7 @@
         <v>25</v>
       </c>
       <c r="I210">
-        <v>5118</v>
+        <v>5255</v>
       </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.25">
@@ -9804,7 +9804,7 @@
         <v>25</v>
       </c>
       <c r="I211">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
@@ -9833,7 +9833,7 @@
         <v>25</v>
       </c>
       <c r="I212">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.25">
@@ -9862,7 +9862,7 @@
         <v>25</v>
       </c>
       <c r="I213">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
@@ -9920,7 +9920,7 @@
         <v>25</v>
       </c>
       <c r="I215">
-        <v>3697</v>
+        <v>3645</v>
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.25">
@@ -9949,7 +9949,7 @@
         <v>25</v>
       </c>
       <c r="I216">
-        <v>3398</v>
+        <v>3444</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.25">
@@ -9978,7 +9978,7 @@
         <v>25</v>
       </c>
       <c r="I217">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.25">
@@ -10036,7 +10036,7 @@
         <v>44</v>
       </c>
       <c r="I219">
-        <v>1400</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.25">
@@ -10065,7 +10065,7 @@
         <v>25</v>
       </c>
       <c r="I220">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.25">
@@ -10094,7 +10094,7 @@
         <v>25</v>
       </c>
       <c r="I221">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.25">
@@ -10123,7 +10123,7 @@
         <v>25</v>
       </c>
       <c r="I222">
-        <v>1249</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.25">
@@ -10152,7 +10152,7 @@
         <v>25</v>
       </c>
       <c r="I223">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.25">
@@ -10239,7 +10239,7 @@
         <v>25</v>
       </c>
       <c r="I226">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.25">
@@ -10268,7 +10268,7 @@
         <v>25</v>
       </c>
       <c r="I227">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.25">
@@ -10384,7 +10384,7 @@
         <v>25</v>
       </c>
       <c r="I231">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.25">
@@ -10413,7 +10413,7 @@
         <v>25</v>
       </c>
       <c r="I232">
-        <v>2380</v>
+        <v>2418</v>
       </c>
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.25">
@@ -10471,7 +10471,7 @@
         <v>25</v>
       </c>
       <c r="I234">
-        <v>3578</v>
+        <v>3571</v>
       </c>
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.25">
@@ -10500,7 +10500,7 @@
         <v>25</v>
       </c>
       <c r="I235">
-        <v>989</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.25">
@@ -10529,7 +10529,7 @@
         <v>25</v>
       </c>
       <c r="I236">
-        <v>15847</v>
+        <v>15894</v>
       </c>
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.25">
@@ -10558,7 +10558,7 @@
         <v>25</v>
       </c>
       <c r="I237">
-        <v>41313</v>
+        <v>41554</v>
       </c>
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.25">
@@ -10587,7 +10587,7 @@
         <v>44</v>
       </c>
       <c r="I238">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.25">
@@ -10616,7 +10616,7 @@
         <v>44</v>
       </c>
       <c r="I239">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.25">
@@ -10645,7 +10645,7 @@
         <v>25</v>
       </c>
       <c r="I240">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.25">
@@ -10674,7 +10674,7 @@
         <v>25</v>
       </c>
       <c r="I241">
-        <v>277</v>
+        <v>288</v>
       </c>
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.25">
@@ -10732,7 +10732,7 @@
         <v>25</v>
       </c>
       <c r="I243">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.25">
@@ -10761,7 +10761,7 @@
         <v>25</v>
       </c>
       <c r="I244">
-        <v>475</v>
+        <v>489</v>
       </c>
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.25">
@@ -10790,7 +10790,7 @@
         <v>25</v>
       </c>
       <c r="I245">
-        <v>1340</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.25">
@@ -10877,7 +10877,7 @@
         <v>25</v>
       </c>
       <c r="I248">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.25">
@@ -11111,7 +11111,7 @@
         <v>993</v>
       </c>
       <c r="B13">
-        <v>41313</v>
+        <v>41554</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -11119,7 +11119,7 @@
         <v>989</v>
       </c>
       <c r="B14">
-        <v>15847</v>
+        <v>15894</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -11127,7 +11127,7 @@
         <v>380</v>
       </c>
       <c r="B15">
-        <v>14968</v>
+        <v>15357</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -11135,7 +11135,7 @@
         <v>669</v>
       </c>
       <c r="B16">
-        <v>10776</v>
+        <v>10629</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -11143,7 +11143,7 @@
         <v>777</v>
       </c>
       <c r="B17">
-        <v>8996</v>
+        <v>9089</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -11151,7 +11151,7 @@
         <v>352</v>
       </c>
       <c r="B18">
-        <v>8795</v>
+        <v>8769</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -11159,7 +11159,7 @@
         <v>201</v>
       </c>
       <c r="B19">
-        <v>8788</v>
+        <v>8731</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -11167,7 +11167,7 @@
         <v>457</v>
       </c>
       <c r="B20">
-        <v>7778</v>
+        <v>7714</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -11175,15 +11175,15 @@
         <v>87</v>
       </c>
       <c r="B21">
-        <v>7238</v>
+        <v>7251</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>497</v>
+        <v>445</v>
       </c>
       <c r="B22">
-        <v>6570</v>
+        <v>6759</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: update geo-ip data - 20250912_144743
📊 Data sync summary:
- Updated at: 2025-09-12 14:47:45 UTC
- Territories: 250
- IP ranges: 258299
- Data size: 41.20MB

🤖 Auto-generated by GitHub Actions
</commit_message>
<xml_diff>
--- a/data/combined-geo-ip-data.xlsx
+++ b/data/combined-geo-ip-data.xlsx
@@ -22,7 +22,7 @@
     <t>Generated at:</t>
   </si>
   <si>
-    <t>2025-08-12T03:16:22.102Z</t>
+    <t>2025-09-12T14:45:57.445Z</t>
   </si>
   <si>
     <t>Metric</t>
@@ -3172,7 +3172,7 @@
     <t>IP Ranges Data Too Large</t>
   </si>
   <si>
-    <t>Total IP ranges: 256807</t>
+    <t>Total IP ranges: 258299</t>
   </si>
   <si>
     <t>The IP ranges data is too large to include in Excel format.</t>
@@ -3661,7 +3661,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>256807</v>
+        <v>258299</v>
       </c>
     </row>
   </sheetData>
@@ -3743,7 +3743,7 @@
         <v>25</v>
       </c>
       <c r="I2">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -3772,7 +3772,7 @@
         <v>25</v>
       </c>
       <c r="I3">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -3801,7 +3801,7 @@
         <v>25</v>
       </c>
       <c r="I4">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -3859,7 +3859,7 @@
         <v>25</v>
       </c>
       <c r="I6">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -3888,7 +3888,7 @@
         <v>25</v>
       </c>
       <c r="I7">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3946,7 +3946,7 @@
         <v>44</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -3975,7 +3975,7 @@
         <v>25</v>
       </c>
       <c r="I10">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -4004,7 +4004,7 @@
         <v>25</v>
       </c>
       <c r="I11">
-        <v>1859</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -4033,7 +4033,7 @@
         <v>25</v>
       </c>
       <c r="I12">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -4091,7 +4091,7 @@
         <v>25</v>
       </c>
       <c r="I14">
-        <v>7238</v>
+        <v>7251</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -4120,7 +4120,7 @@
         <v>25</v>
       </c>
       <c r="I15">
-        <v>2313</v>
+        <v>2322</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -4149,7 +4149,7 @@
         <v>25</v>
       </c>
       <c r="I16">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -4178,7 +4178,7 @@
         <v>25</v>
       </c>
       <c r="I17">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -4207,7 +4207,7 @@
         <v>25</v>
       </c>
       <c r="I18">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -4236,7 +4236,7 @@
         <v>25</v>
       </c>
       <c r="I19">
-        <v>1973</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -4265,7 +4265,7 @@
         <v>25</v>
       </c>
       <c r="I20">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -4294,7 +4294,7 @@
         <v>25</v>
       </c>
       <c r="I21">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -4323,7 +4323,7 @@
         <v>25</v>
       </c>
       <c r="I22">
-        <v>4930</v>
+        <v>5035</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -4352,7 +4352,7 @@
         <v>25</v>
       </c>
       <c r="I23">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -4410,7 +4410,7 @@
         <v>44</v>
       </c>
       <c r="I25">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -4439,7 +4439,7 @@
         <v>25</v>
       </c>
       <c r="I26">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -4468,7 +4468,7 @@
         <v>25</v>
       </c>
       <c r="I27">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -4497,7 +4497,7 @@
         <v>25</v>
       </c>
       <c r="I28">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -4526,7 +4526,7 @@
         <v>25</v>
       </c>
       <c r="I29">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -4584,7 +4584,7 @@
         <v>25</v>
       </c>
       <c r="I31">
-        <v>4802</v>
+        <v>4790</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -4642,7 +4642,7 @@
         <v>44</v>
       </c>
       <c r="I33">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -4671,7 +4671,7 @@
         <v>25</v>
       </c>
       <c r="I34">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -4729,7 +4729,7 @@
         <v>25</v>
       </c>
       <c r="I36">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -4758,7 +4758,7 @@
         <v>25</v>
       </c>
       <c r="I37">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -4787,7 +4787,7 @@
         <v>25</v>
       </c>
       <c r="I38">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -4845,7 +4845,7 @@
         <v>25</v>
       </c>
       <c r="I40">
-        <v>8788</v>
+        <v>8731</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -4903,7 +4903,7 @@
         <v>44</v>
       </c>
       <c r="I42">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -4932,7 +4932,7 @@
         <v>44</v>
       </c>
       <c r="I43">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -4961,7 +4961,7 @@
         <v>25</v>
       </c>
       <c r="I44">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -5019,7 +5019,7 @@
         <v>25</v>
       </c>
       <c r="I46">
-        <v>1014</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -5048,7 +5048,7 @@
         <v>25</v>
       </c>
       <c r="I47">
-        <v>4422</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -5135,7 +5135,7 @@
         <v>25</v>
       </c>
       <c r="I50">
-        <v>1039</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -5193,7 +5193,7 @@
         <v>25</v>
       </c>
       <c r="I52">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -5222,7 +5222,7 @@
         <v>44</v>
       </c>
       <c r="I53">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -5251,7 +5251,7 @@
         <v>25</v>
       </c>
       <c r="I54">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -5280,7 +5280,7 @@
         <v>25</v>
       </c>
       <c r="I55">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -5338,7 +5338,7 @@
         <v>44</v>
       </c>
       <c r="I57">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -5367,7 +5367,7 @@
         <v>25</v>
       </c>
       <c r="I58">
-        <v>337</v>
+        <v>342</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -5396,7 +5396,7 @@
         <v>25</v>
       </c>
       <c r="I59">
-        <v>1883</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -5425,7 +5425,7 @@
         <v>25</v>
       </c>
       <c r="I60">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -5454,7 +5454,7 @@
         <v>25</v>
       </c>
       <c r="I61">
-        <v>1601</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -5483,7 +5483,7 @@
         <v>25</v>
       </c>
       <c r="I62">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -5512,7 +5512,7 @@
         <v>25</v>
       </c>
       <c r="I63">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -5541,7 +5541,7 @@
         <v>25</v>
       </c>
       <c r="I64">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -5570,7 +5570,7 @@
         <v>25</v>
       </c>
       <c r="I65">
-        <v>465</v>
+        <v>448</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -5599,7 +5599,7 @@
         <v>25</v>
       </c>
       <c r="I66">
-        <v>298</v>
+        <v>310</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -5628,7 +5628,7 @@
         <v>25</v>
       </c>
       <c r="I67">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -5686,7 +5686,7 @@
         <v>25</v>
       </c>
       <c r="I69">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -5715,7 +5715,7 @@
         <v>25</v>
       </c>
       <c r="I70">
-        <v>658</v>
+        <v>676</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -5889,7 +5889,7 @@
         <v>25</v>
       </c>
       <c r="I76">
-        <v>1845</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -5918,7 +5918,7 @@
         <v>25</v>
       </c>
       <c r="I77">
-        <v>8795</v>
+        <v>8769</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -5976,7 +5976,7 @@
         <v>44</v>
       </c>
       <c r="I79">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -6034,7 +6034,7 @@
         <v>25</v>
       </c>
       <c r="I81">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -6092,7 +6092,7 @@
         <v>25</v>
       </c>
       <c r="I83">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -6121,7 +6121,7 @@
         <v>25</v>
       </c>
       <c r="I84">
-        <v>14968</v>
+        <v>15357</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -6150,7 +6150,7 @@
         <v>25</v>
       </c>
       <c r="I85">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -6208,7 +6208,7 @@
         <v>25</v>
       </c>
       <c r="I87">
-        <v>685</v>
+        <v>695</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -6237,7 +6237,7 @@
         <v>44</v>
       </c>
       <c r="I88">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -6266,7 +6266,7 @@
         <v>25</v>
       </c>
       <c r="I89">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -6295,7 +6295,7 @@
         <v>44</v>
       </c>
       <c r="I90">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -6324,7 +6324,7 @@
         <v>44</v>
       </c>
       <c r="I91">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -6353,7 +6353,7 @@
         <v>25</v>
       </c>
       <c r="I92">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -6382,7 +6382,7 @@
         <v>44</v>
       </c>
       <c r="I93">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -6411,7 +6411,7 @@
         <v>25</v>
       </c>
       <c r="I94">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -6440,7 +6440,7 @@
         <v>25</v>
       </c>
       <c r="I95">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -6469,7 +6469,7 @@
         <v>25</v>
       </c>
       <c r="I96">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -6498,7 +6498,7 @@
         <v>25</v>
       </c>
       <c r="I97">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -6556,7 +6556,7 @@
         <v>25</v>
       </c>
       <c r="I99">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -6585,7 +6585,7 @@
         <v>44</v>
       </c>
       <c r="I100">
-        <v>6500</v>
+        <v>6759</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -6614,7 +6614,7 @@
         <v>25</v>
       </c>
       <c r="I101">
-        <v>937</v>
+        <v>922</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -6672,7 +6672,7 @@
         <v>25</v>
       </c>
       <c r="I103">
-        <v>7778</v>
+        <v>7714</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -6701,7 +6701,7 @@
         <v>25</v>
       </c>
       <c r="I104">
-        <v>4407</v>
+        <v>4474</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
@@ -6730,7 +6730,7 @@
         <v>25</v>
       </c>
       <c r="I105">
-        <v>1605</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
@@ -6759,7 +6759,7 @@
         <v>25</v>
       </c>
       <c r="I106">
-        <v>383</v>
+        <v>388</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -6788,7 +6788,7 @@
         <v>25</v>
       </c>
       <c r="I107">
-        <v>2220</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -6817,7 +6817,7 @@
         <v>44</v>
       </c>
       <c r="I108">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
@@ -6846,7 +6846,7 @@
         <v>25</v>
       </c>
       <c r="I109">
-        <v>1178</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -6875,7 +6875,7 @@
         <v>25</v>
       </c>
       <c r="I110">
-        <v>4977</v>
+        <v>5032</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
@@ -6904,7 +6904,7 @@
         <v>25</v>
       </c>
       <c r="I111">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -6933,7 +6933,7 @@
         <v>25</v>
       </c>
       <c r="I112">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
@@ -6962,7 +6962,7 @@
         <v>25</v>
       </c>
       <c r="I113">
-        <v>6570</v>
+        <v>6603</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
@@ -6991,7 +6991,7 @@
         <v>44</v>
       </c>
       <c r="I114">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -7020,7 +7020,7 @@
         <v>25</v>
       </c>
       <c r="I115">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -7049,7 +7049,7 @@
         <v>25</v>
       </c>
       <c r="I116">
-        <v>893</v>
+        <v>907</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -7078,7 +7078,7 @@
         <v>25</v>
       </c>
       <c r="I117">
-        <v>488</v>
+        <v>492</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -7107,7 +7107,7 @@
         <v>25</v>
       </c>
       <c r="I118">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -7165,7 +7165,7 @@
         <v>25</v>
       </c>
       <c r="I120">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -7194,7 +7194,7 @@
         <v>25</v>
       </c>
       <c r="I121">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
@@ -7223,7 +7223,7 @@
         <v>25</v>
       </c>
       <c r="I122">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
@@ -7252,7 +7252,7 @@
         <v>25</v>
       </c>
       <c r="I123">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
@@ -7281,7 +7281,7 @@
         <v>25</v>
       </c>
       <c r="I124">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
@@ -7339,7 +7339,7 @@
         <v>25</v>
       </c>
       <c r="I126">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
@@ -7397,7 +7397,7 @@
         <v>25</v>
       </c>
       <c r="I128">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -7426,7 +7426,7 @@
         <v>25</v>
       </c>
       <c r="I129">
-        <v>894</v>
+        <v>857</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -7455,7 +7455,7 @@
         <v>25</v>
       </c>
       <c r="I130">
-        <v>554</v>
+        <v>545</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
@@ -7513,7 +7513,7 @@
         <v>25</v>
       </c>
       <c r="I132">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
@@ -7542,7 +7542,7 @@
         <v>25</v>
       </c>
       <c r="I133">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
@@ -7571,7 +7571,7 @@
         <v>25</v>
       </c>
       <c r="I134">
-        <v>1433</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
@@ -7600,7 +7600,7 @@
         <v>25</v>
       </c>
       <c r="I135">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
@@ -7629,7 +7629,7 @@
         <v>25</v>
       </c>
       <c r="I136">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
@@ -7658,7 +7658,7 @@
         <v>25</v>
       </c>
       <c r="I137">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
@@ -7687,7 +7687,7 @@
         <v>25</v>
       </c>
       <c r="I138">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
@@ -7832,7 +7832,7 @@
         <v>25</v>
       </c>
       <c r="I143">
-        <v>1611</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
@@ -7861,7 +7861,7 @@
         <v>25</v>
       </c>
       <c r="I144">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
@@ -7890,7 +7890,7 @@
         <v>25</v>
       </c>
       <c r="I145">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
@@ -7919,7 +7919,7 @@
         <v>25</v>
       </c>
       <c r="I146">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
@@ -7977,7 +7977,7 @@
         <v>25</v>
       </c>
       <c r="I148">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
@@ -8006,7 +8006,7 @@
         <v>44</v>
       </c>
       <c r="I149">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
@@ -8035,7 +8035,7 @@
         <v>25</v>
       </c>
       <c r="I150">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
@@ -8064,7 +8064,7 @@
         <v>25</v>
       </c>
       <c r="I151">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
@@ -8093,7 +8093,7 @@
         <v>25</v>
       </c>
       <c r="I152">
-        <v>287</v>
+        <v>294</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
@@ -8122,7 +8122,7 @@
         <v>25</v>
       </c>
       <c r="I153">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
@@ -8180,7 +8180,7 @@
         <v>25</v>
       </c>
       <c r="I155">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
@@ -8209,7 +8209,7 @@
         <v>25</v>
       </c>
       <c r="I156">
-        <v>10776</v>
+        <v>10629</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
@@ -8238,7 +8238,7 @@
         <v>44</v>
       </c>
       <c r="I157">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
@@ -8267,7 +8267,7 @@
         <v>25</v>
       </c>
       <c r="I158">
-        <v>1504</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
@@ -8296,7 +8296,7 @@
         <v>25</v>
       </c>
       <c r="I159">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
@@ -8354,7 +8354,7 @@
         <v>25</v>
       </c>
       <c r="I161">
-        <v>507</v>
+        <v>522</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
@@ -8470,7 +8470,7 @@
         <v>25</v>
       </c>
       <c r="I165">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
@@ -8499,7 +8499,7 @@
         <v>44</v>
       </c>
       <c r="I166">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
@@ -8528,7 +8528,7 @@
         <v>25</v>
       </c>
       <c r="I167">
-        <v>1657</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
@@ -8557,7 +8557,7 @@
         <v>25</v>
       </c>
       <c r="I168">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
@@ -8586,7 +8586,7 @@
         <v>25</v>
       </c>
       <c r="I169">
-        <v>841</v>
+        <v>847</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
@@ -8615,7 +8615,7 @@
         <v>25</v>
       </c>
       <c r="I170">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
@@ -8644,7 +8644,7 @@
         <v>44</v>
       </c>
       <c r="I171">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
@@ -8673,7 +8673,7 @@
         <v>25</v>
       </c>
       <c r="I172">
-        <v>325</v>
+        <v>316</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
@@ -8702,7 +8702,7 @@
         <v>25</v>
       </c>
       <c r="I173">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
@@ -8731,7 +8731,7 @@
         <v>25</v>
       </c>
       <c r="I174">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
@@ -8760,7 +8760,7 @@
         <v>25</v>
       </c>
       <c r="I175">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
@@ -8789,7 +8789,7 @@
         <v>25</v>
       </c>
       <c r="I176">
-        <v>1451</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
@@ -8847,7 +8847,7 @@
         <v>25</v>
       </c>
       <c r="I178">
-        <v>4916</v>
+        <v>4923</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
@@ -8876,7 +8876,7 @@
         <v>25</v>
       </c>
       <c r="I179">
-        <v>649</v>
+        <v>661</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
@@ -8905,7 +8905,7 @@
         <v>44</v>
       </c>
       <c r="I180">
-        <v>374</v>
+        <v>357</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
@@ -8934,7 +8934,7 @@
         <v>25</v>
       </c>
       <c r="I181">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
@@ -8963,7 +8963,7 @@
         <v>25</v>
       </c>
       <c r="I182">
-        <v>2469</v>
+        <v>2426</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
@@ -8992,7 +8992,7 @@
         <v>25</v>
       </c>
       <c r="I183">
-        <v>8996</v>
+        <v>9089</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
@@ -9021,7 +9021,7 @@
         <v>25</v>
       </c>
       <c r="I184">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
@@ -9050,7 +9050,7 @@
         <v>44</v>
       </c>
       <c r="I185">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
@@ -9079,7 +9079,7 @@
         <v>44</v>
       </c>
       <c r="I186">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
@@ -9137,7 +9137,7 @@
         <v>25</v>
       </c>
       <c r="I188">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
@@ -9195,7 +9195,7 @@
         <v>44</v>
       </c>
       <c r="I190">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.25">
@@ -9253,7 +9253,7 @@
         <v>25</v>
       </c>
       <c r="I192">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
@@ -9282,7 +9282,7 @@
         <v>25</v>
       </c>
       <c r="I193">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
@@ -9340,7 +9340,7 @@
         <v>25</v>
       </c>
       <c r="I195">
-        <v>885</v>
+        <v>920</v>
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.25">
@@ -9369,7 +9369,7 @@
         <v>25</v>
       </c>
       <c r="I196">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.25">
@@ -9398,7 +9398,7 @@
         <v>25</v>
       </c>
       <c r="I197">
-        <v>574</v>
+        <v>578</v>
       </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.25">
@@ -9427,7 +9427,7 @@
         <v>25</v>
       </c>
       <c r="I198">
-        <v>336</v>
+        <v>296</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.25">
@@ -9456,7 +9456,7 @@
         <v>25</v>
       </c>
       <c r="I199">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.25">
@@ -9485,7 +9485,7 @@
         <v>25</v>
       </c>
       <c r="I200">
-        <v>4872</v>
+        <v>4906</v>
       </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">
@@ -9543,7 +9543,7 @@
         <v>25</v>
       </c>
       <c r="I202">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.25">
@@ -9572,7 +9572,7 @@
         <v>25</v>
       </c>
       <c r="I203">
-        <v>574</v>
+        <v>603</v>
       </c>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
@@ -9601,7 +9601,7 @@
         <v>25</v>
       </c>
       <c r="I204">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.25">
@@ -9630,7 +9630,7 @@
         <v>25</v>
       </c>
       <c r="I205">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.25">
@@ -9659,7 +9659,7 @@
         <v>25</v>
       </c>
       <c r="I206">
-        <v>2316</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.25">
@@ -9717,7 +9717,7 @@
         <v>25</v>
       </c>
       <c r="I208">
-        <v>2275</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.25">
@@ -9746,7 +9746,7 @@
         <v>25</v>
       </c>
       <c r="I209">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.25">
@@ -9775,7 +9775,7 @@
         <v>25</v>
       </c>
       <c r="I210">
-        <v>5118</v>
+        <v>5255</v>
       </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.25">
@@ -9804,7 +9804,7 @@
         <v>25</v>
       </c>
       <c r="I211">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
@@ -9833,7 +9833,7 @@
         <v>25</v>
       </c>
       <c r="I212">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.25">
@@ -9862,7 +9862,7 @@
         <v>25</v>
       </c>
       <c r="I213">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
@@ -9920,7 +9920,7 @@
         <v>25</v>
       </c>
       <c r="I215">
-        <v>3697</v>
+        <v>3645</v>
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.25">
@@ -9949,7 +9949,7 @@
         <v>25</v>
       </c>
       <c r="I216">
-        <v>3398</v>
+        <v>3444</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.25">
@@ -9978,7 +9978,7 @@
         <v>25</v>
       </c>
       <c r="I217">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.25">
@@ -10036,7 +10036,7 @@
         <v>44</v>
       </c>
       <c r="I219">
-        <v>1400</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.25">
@@ -10065,7 +10065,7 @@
         <v>25</v>
       </c>
       <c r="I220">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.25">
@@ -10094,7 +10094,7 @@
         <v>25</v>
       </c>
       <c r="I221">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.25">
@@ -10123,7 +10123,7 @@
         <v>25</v>
       </c>
       <c r="I222">
-        <v>1249</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.25">
@@ -10152,7 +10152,7 @@
         <v>25</v>
       </c>
       <c r="I223">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.25">
@@ -10239,7 +10239,7 @@
         <v>25</v>
       </c>
       <c r="I226">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.25">
@@ -10268,7 +10268,7 @@
         <v>25</v>
       </c>
       <c r="I227">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.25">
@@ -10384,7 +10384,7 @@
         <v>25</v>
       </c>
       <c r="I231">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.25">
@@ -10413,7 +10413,7 @@
         <v>25</v>
       </c>
       <c r="I232">
-        <v>2380</v>
+        <v>2418</v>
       </c>
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.25">
@@ -10471,7 +10471,7 @@
         <v>25</v>
       </c>
       <c r="I234">
-        <v>3578</v>
+        <v>3571</v>
       </c>
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.25">
@@ -10500,7 +10500,7 @@
         <v>25</v>
       </c>
       <c r="I235">
-        <v>989</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.25">
@@ -10529,7 +10529,7 @@
         <v>25</v>
       </c>
       <c r="I236">
-        <v>15847</v>
+        <v>15894</v>
       </c>
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.25">
@@ -10558,7 +10558,7 @@
         <v>25</v>
       </c>
       <c r="I237">
-        <v>41313</v>
+        <v>41554</v>
       </c>
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.25">
@@ -10587,7 +10587,7 @@
         <v>44</v>
       </c>
       <c r="I238">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.25">
@@ -10616,7 +10616,7 @@
         <v>44</v>
       </c>
       <c r="I239">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.25">
@@ -10645,7 +10645,7 @@
         <v>25</v>
       </c>
       <c r="I240">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.25">
@@ -10674,7 +10674,7 @@
         <v>25</v>
       </c>
       <c r="I241">
-        <v>277</v>
+        <v>288</v>
       </c>
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.25">
@@ -10732,7 +10732,7 @@
         <v>25</v>
       </c>
       <c r="I243">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.25">
@@ -10761,7 +10761,7 @@
         <v>25</v>
       </c>
       <c r="I244">
-        <v>475</v>
+        <v>489</v>
       </c>
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.25">
@@ -10790,7 +10790,7 @@
         <v>25</v>
       </c>
       <c r="I245">
-        <v>1340</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.25">
@@ -10877,7 +10877,7 @@
         <v>25</v>
       </c>
       <c r="I248">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.25">
@@ -11111,7 +11111,7 @@
         <v>993</v>
       </c>
       <c r="B13">
-        <v>41313</v>
+        <v>41554</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -11119,7 +11119,7 @@
         <v>989</v>
       </c>
       <c r="B14">
-        <v>15847</v>
+        <v>15894</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -11127,7 +11127,7 @@
         <v>380</v>
       </c>
       <c r="B15">
-        <v>14968</v>
+        <v>15357</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -11135,7 +11135,7 @@
         <v>669</v>
       </c>
       <c r="B16">
-        <v>10776</v>
+        <v>10629</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -11143,7 +11143,7 @@
         <v>777</v>
       </c>
       <c r="B17">
-        <v>8996</v>
+        <v>9089</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -11151,7 +11151,7 @@
         <v>352</v>
       </c>
       <c r="B18">
-        <v>8795</v>
+        <v>8769</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -11159,7 +11159,7 @@
         <v>201</v>
       </c>
       <c r="B19">
-        <v>8788</v>
+        <v>8731</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -11167,7 +11167,7 @@
         <v>457</v>
       </c>
       <c r="B20">
-        <v>7778</v>
+        <v>7714</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -11175,15 +11175,15 @@
         <v>87</v>
       </c>
       <c r="B21">
-        <v>7238</v>
+        <v>7251</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>497</v>
+        <v>445</v>
       </c>
       <c r="B22">
-        <v>6570</v>
+        <v>6759</v>
       </c>
     </row>
   </sheetData>

</xml_diff>